<commit_message>
Update readme and header template to include group option
</commit_message>
<xml_diff>
--- a/quarterlyReports/header_file_template.xlsx
+++ b/quarterlyReports/header_file_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mayalapp/Documents/coding_projects/dad_data_project/quarterlyReports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9D79CA-6984-3349-A0A5-18158699EF81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F10C2A79-5A57-6D48-8C21-CA127FF0EA3C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="13960" activeTab="1" xr2:uid="{A3C09648-A85F-004C-88D6-616841BE841B}"/>
+    <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="13960" xr2:uid="{A3C09648-A85F-004C-88D6-616841BE841B}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Screened patients: Patients that received a mammogram during the 2 years prior to the end of the reporting period.</t>
   </si>
@@ -62,6 +62,15 @@
   </si>
   <si>
     <t>Additional notes if needed - can be on multiple lines</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group category used to break data into different plots (e.g. site, provider, patient demographics, etc.)  </t>
   </si>
 </sst>
 </file>
@@ -434,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3305214C-55D9-ED4E-A364-E0362E1B513C}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -472,6 +481,14 @@
         <v>8</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -479,10 +496,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E731B5D-8C6F-4B45-B462-14B88FDFFF33}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -512,6 +529,14 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>